<commit_message>
min Year | max Year
</commit_message>
<xml_diff>
--- a/excel/modelo_linha_do_tempo.xlsx
+++ b/excel/modelo_linha_do_tempo.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>n/a</t>
   </si>
@@ -104,6 +104,24 @@
   </si>
   <si>
     <t>victor Aids</t>
+  </si>
+  <si>
+    <t>DiaI</t>
+  </si>
+  <si>
+    <t>MêsI</t>
+  </si>
+  <si>
+    <t>AnoI</t>
+  </si>
+  <si>
+    <t>DiaF</t>
+  </si>
+  <si>
+    <t>MêsF</t>
+  </si>
+  <si>
+    <t>AnoF</t>
   </si>
 </sst>
 </file>
@@ -179,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -203,9 +221,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -215,12 +231,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -228,9 +257,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -244,12 +270,375 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1822,11 +2211,11 @@
         </c:dLbls>
         <c:gapWidth val="10"/>
         <c:overlap val="100"/>
-        <c:axId val="360080320"/>
-        <c:axId val="396685352"/>
+        <c:axId val="350927144"/>
+        <c:axId val="351281792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="360080320"/>
+        <c:axId val="350927144"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1880,7 +2269,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="396685352"/>
+        <c:crossAx val="351281792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1888,7 +2277,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="396685352"/>
+        <c:axId val="351281792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43466"/>
@@ -1938,7 +2327,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360080320"/>
+        <c:crossAx val="350927144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="366"/>
@@ -1989,23 +2378,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{52BF227D-3AC3-4B5A-88A9-8F410E929E4B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52BF227D-3AC3-4B5A-88A9-8F410E929E4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2026,6 +2415,48 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:G20" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A1:G20"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Evento" dataDxfId="11"/>
+    <tableColumn id="2" name="Data inicial" dataDxfId="10" dataCellStyle="Vírgula"/>
+    <tableColumn id="3" name="Duração em dias" dataDxfId="9" dataCellStyle="Vírgula">
+      <calculatedColumnFormula>D2-B2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Data final" dataDxfId="8" dataCellStyle="Vírgula"/>
+    <tableColumn id="5" name="DiaI" dataDxfId="6">
+      <calculatedColumnFormula>DAY(Tabela1[[#This Row],[Data inicial]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="MêsI" dataDxfId="5">
+      <calculatedColumnFormula>MONTH(Tabela1[[#This Row],[Data inicial]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="AnoI" dataDxfId="7">
+      <calculatedColumnFormula>YEAR(Tabela1[[#This Row],[Data inicial]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="H1:J20" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
+  <autoFilter ref="H1:J20"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="DiaF" dataDxfId="2">
+      <calculatedColumnFormula>DAY(Tabela1[[#This Row],[Data final]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="MêsF" dataDxfId="1">
+      <calculatedColumnFormula>MONTH(Tabela1[[#This Row],[Data final]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="AnoF" dataDxfId="0">
+      <calculatedColumnFormula>YEAR(Tabela1[[#This Row],[Data final]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2294,317 +2725,802 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="17.140625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
+    <col min="8" max="10" width="10.28515625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="E1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>41845</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <f>D2-B2</f>
         <v>1194</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>43039</v>
       </c>
+      <c r="E2" s="9">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>25</v>
+      </c>
+      <c r="F2" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>7</v>
+      </c>
+      <c r="G2" s="10">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2014</v>
+      </c>
+      <c r="H2" s="2">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>31</v>
+      </c>
+      <c r="I2" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>10</v>
+      </c>
+      <c r="J2" s="2">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>2017</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>41845</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <f t="shared" ref="C3:C11" si="0">D3-B3</f>
         <v>1194</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>43039</v>
       </c>
+      <c r="E3" s="9">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>25</v>
+      </c>
+      <c r="F3" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>7</v>
+      </c>
+      <c r="G3" s="10">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2014</v>
+      </c>
+      <c r="H3" s="2">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>31</v>
+      </c>
+      <c r="I3" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>10</v>
+      </c>
+      <c r="J3" s="2">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>2017</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>42248</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <f t="shared" si="0"/>
         <v>791</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>43039</v>
       </c>
+      <c r="E4" s="9">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>9</v>
+      </c>
+      <c r="G4" s="10">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2015</v>
+      </c>
+      <c r="H4" s="2">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>31</v>
+      </c>
+      <c r="I4" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>10</v>
+      </c>
+      <c r="J4" s="2">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>2017</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:10" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>42371</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <f t="shared" si="0"/>
         <v>668</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>43039</v>
       </c>
+      <c r="E5" s="9">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="10">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2016</v>
+      </c>
+      <c r="H5" s="2">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>31</v>
+      </c>
+      <c r="I5" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>10</v>
+      </c>
+      <c r="J5" s="2">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>2017</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:10" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>41845</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <f t="shared" si="0"/>
         <v>1194</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>43039</v>
       </c>
+      <c r="E6" s="9">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>25</v>
+      </c>
+      <c r="F6" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>7</v>
+      </c>
+      <c r="G6" s="10">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2014</v>
+      </c>
+      <c r="H6" s="2">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>31</v>
+      </c>
+      <c r="I6" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>10</v>
+      </c>
+      <c r="J6" s="2">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>2017</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:10" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>41883</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <f t="shared" si="0"/>
         <v>1156</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>43039</v>
       </c>
+      <c r="E7" s="9">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>9</v>
+      </c>
+      <c r="G7" s="10">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2014</v>
+      </c>
+      <c r="H7" s="2">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>31</v>
+      </c>
+      <c r="I7" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>10</v>
+      </c>
+      <c r="J7" s="2">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>2017</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:10" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>41640</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <f t="shared" si="0"/>
         <v>1399</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>43039</v>
       </c>
+      <c r="E8" s="9">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="10">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2014</v>
+      </c>
+      <c r="H8" s="2">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>31</v>
+      </c>
+      <c r="I8" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>10</v>
+      </c>
+      <c r="J8" s="2">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>2017</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:10" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>41845</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <f t="shared" si="0"/>
         <v>1194</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>43039</v>
       </c>
+      <c r="E9" s="9">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>25</v>
+      </c>
+      <c r="F9" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>7</v>
+      </c>
+      <c r="G9" s="10">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2014</v>
+      </c>
+      <c r="H9" s="2">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>31</v>
+      </c>
+      <c r="I9" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>10</v>
+      </c>
+      <c r="J9" s="2">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>2017</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:10" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>41845</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <f t="shared" si="0"/>
         <v>1194</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>43039</v>
       </c>
+      <c r="E10" s="9">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>25</v>
+      </c>
+      <c r="F10" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>7</v>
+      </c>
+      <c r="G10" s="10">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2014</v>
+      </c>
+      <c r="H10" s="2">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>31</v>
+      </c>
+      <c r="I10" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>10</v>
+      </c>
+      <c r="J10" s="2">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>2017</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:10" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>42309</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <f t="shared" si="0"/>
         <v>730</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>43039</v>
       </c>
+      <c r="E11" s="9">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>11</v>
+      </c>
+      <c r="G11" s="10">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2015</v>
+      </c>
+      <c r="H11" s="2">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>31</v>
+      </c>
+      <c r="I11" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>10</v>
+      </c>
+      <c r="J11" s="2">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>2017</v>
+      </c>
     </row>
-    <row r="12" spans="1:4" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:10" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>41641</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <f>D12-B12</f>
         <v>1398</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>43039</v>
       </c>
+      <c r="E12" s="9">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2</v>
+      </c>
+      <c r="F12" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="10">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2014</v>
+      </c>
+      <c r="H12" s="2">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>31</v>
+      </c>
+      <c r="I12" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>10</v>
+      </c>
+      <c r="J12" s="2">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>2017</v>
+      </c>
     </row>
-    <row r="13" spans="1:4" s="2" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:10" s="2" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6">
+      <c r="B13" s="4"/>
+      <c r="C13" s="5">
         <f>D13-B13</f>
         <v>0</v>
       </c>
-      <c r="D13" s="5"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="9">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="10">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>1900</v>
+      </c>
+      <c r="H13" s="2">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>1</v>
+      </c>
+      <c r="J13" s="2">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>1900</v>
+      </c>
     </row>
-    <row r="14" spans="1:4" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:10" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>41560</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <f>D14-B14</f>
         <v>1479</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>43039</v>
       </c>
+      <c r="E14" s="9">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>13</v>
+      </c>
+      <c r="F14" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>10</v>
+      </c>
+      <c r="G14" s="10">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2013</v>
+      </c>
+      <c r="H14" s="2">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>31</v>
+      </c>
+      <c r="I14" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>10</v>
+      </c>
+      <c r="J14" s="2">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>2017</v>
+      </c>
     </row>
-    <row r="15" spans="1:4" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:10" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>41183</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <f t="shared" ref="C15:C18" si="1">D15-B15</f>
         <v>1856</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>43039</v>
       </c>
+      <c r="E15" s="9">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>10</v>
+      </c>
+      <c r="G15" s="10">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2012</v>
+      </c>
+      <c r="H15" s="2">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>31</v>
+      </c>
+      <c r="I15" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>10</v>
+      </c>
+      <c r="J15" s="2">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>2017</v>
+      </c>
     </row>
-    <row r="16" spans="1:4" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:10" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>41276</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <f t="shared" si="1"/>
         <v>1763</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>43039</v>
       </c>
+      <c r="E16" s="9">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2</v>
+      </c>
+      <c r="F16" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>1</v>
+      </c>
+      <c r="G16" s="10">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2013</v>
+      </c>
+      <c r="H16" s="2">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>31</v>
+      </c>
+      <c r="I16" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>10</v>
+      </c>
+      <c r="J16" s="2">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>2017</v>
+      </c>
     </row>
-    <row r="17" spans="1:4" s="2" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:10" s="2" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="6" t="e">
+      <c r="C17" s="5" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="E17" s="9" t="e">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F17" s="2" t="e">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G17" s="10" t="e">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H17" s="2" t="e">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I17" s="2" t="e">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J17" s="2" t="e">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
-    <row r="18" spans="1:4" s="2" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:10" s="2" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="6" t="e">
+      <c r="C18" s="5" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="E18" s="9" t="e">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F18" s="2" t="e">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G18" s="10" t="e">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H18" s="2" t="e">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I18" s="2" t="e">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J18" s="2" t="e">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
-    <row r="19" spans="1:4" s="2" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:10" s="2" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6">
+      <c r="B19" s="4"/>
+      <c r="C19" s="5">
         <f>D19-B19</f>
         <v>0</v>
       </c>
-      <c r="D19" s="5"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="9">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>1</v>
+      </c>
+      <c r="G19" s="10">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>1900</v>
+      </c>
+      <c r="H19" s="2">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>1</v>
+      </c>
+      <c r="J19" s="2">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>1900</v>
+      </c>
     </row>
-    <row r="20" spans="1:4" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:10" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>41276</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <f t="shared" ref="C20" si="2">D20-B20</f>
         <v>1763</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <v>43039</v>
       </c>
+      <c r="E20" s="9">
+        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2</v>
+      </c>
+      <c r="F20" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="10">
+        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
+        <v>2013</v>
+      </c>
+      <c r="H20" s="2">
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>31</v>
+      </c>
+      <c r="I20" s="2">
+        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
+        <v>10</v>
+      </c>
+      <c r="J20" s="2">
+        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D11"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="2">
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
create borady by excell | Customize color
</commit_message>
<xml_diff>
--- a/excel/modelo_linha_do_tempo.xlsx
+++ b/excel/modelo_linha_do_tempo.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>E</t>
   </si>
@@ -117,6 +117,27 @@
   <si>
     <t>Robando e Mentindo</t>
   </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>146,208,80</t>
+  </si>
+  <si>
+    <t>244,176,132</t>
+  </si>
+  <si>
+    <t>112,48,160</t>
+  </si>
+  <si>
+    <t>174,170,170</t>
+  </si>
+  <si>
+    <t>255,217,102</t>
+  </si>
+  <si>
+    <t>255,0,0</t>
+  </si>
 </sst>
 </file>
 
@@ -125,7 +146,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,8 +197,20 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,6 +220,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0000CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -243,7 +312,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -286,15 +355,39 @@
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="25">
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -304,50 +397,12 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color auto="1"/>
+        <color theme="1"/>
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -552,6 +607,63 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1186,40 +1298,40 @@
                   <c:v>1194</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1175</c:v>
+                  <c:v>810</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>791</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>668</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1194</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1156</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1399</c:v>
+                  <c:v>607</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1194</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1194</c:v>
+                  <c:v>921</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>730</c:v>
+                  <c:v>373</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1763</c:v>
+                  <c:v>1610</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1194</c:v>
+                  <c:v>829</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1194</c:v>
+                  <c:v>1477</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1460,40 +1572,40 @@
                   <c:v>1194</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1175</c:v>
+                  <c:v>810</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>791</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>668</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1194</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1156</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1399</c:v>
+                  <c:v>607</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1194</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1194</c:v>
+                  <c:v>921</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>730</c:v>
+                  <c:v>373</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1763</c:v>
+                  <c:v>1610</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1194</c:v>
+                  <c:v>829</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1194</c:v>
+                  <c:v>1477</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1734,40 +1846,40 @@
                   <c:v>1194</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1175</c:v>
+                  <c:v>810</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>791</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>668</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1194</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1156</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1399</c:v>
+                  <c:v>607</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1194</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1194</c:v>
+                  <c:v>921</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>730</c:v>
+                  <c:v>373</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1763</c:v>
+                  <c:v>1610</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1194</c:v>
+                  <c:v>829</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1194</c:v>
+                  <c:v>1477</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2297,40 +2409,40 @@
                   <c:v>1194</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1175</c:v>
+                  <c:v>810</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>791</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>668</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1194</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1156</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1399</c:v>
+                  <c:v>607</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1194</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1194</c:v>
+                  <c:v>921</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>730</c:v>
+                  <c:v>373</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1763</c:v>
+                  <c:v>1610</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1194</c:v>
+                  <c:v>829</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1194</c:v>
+                  <c:v>1477</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2351,11 +2463,11 @@
         </c:dLbls>
         <c:gapWidth val="10"/>
         <c:overlap val="100"/>
-        <c:axId val="406992192"/>
-        <c:axId val="406992576"/>
+        <c:axId val="121040080"/>
+        <c:axId val="351978816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="406992192"/>
+        <c:axId val="121040080"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2409,7 +2521,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="406992576"/>
+        <c:crossAx val="351978816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2417,7 +2529,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="406992576"/>
+        <c:axId val="351978816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43466"/>
@@ -2467,7 +2579,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="406992192"/>
+        <c:crossAx val="121040080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="366"/>
@@ -2518,23 +2630,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>514350</xdr:rowOff>
+      <xdr:rowOff>257175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52BF227D-3AC3-4B5A-88A9-8F410E929E4B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{52BF227D-3AC3-4B5A-88A9-8F410E929E4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2558,23 +2670,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:H20" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:H20" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
   <autoFilter ref="A1:H20"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Evento" dataDxfId="20" totalsRowDxfId="19"/>
-    <tableColumn id="2" name="Data inicial" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Vírgula"/>
-    <tableColumn id="3" name="Duração em dias" dataDxfId="16" totalsRowDxfId="15" dataCellStyle="Vírgula">
+    <tableColumn id="1" name="Evento" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="2" name="Data inicial" dataDxfId="19" totalsRowDxfId="18" dataCellStyle="Vírgula"/>
+    <tableColumn id="3" name="Duração em dias" dataDxfId="17" totalsRowDxfId="16" dataCellStyle="Vírgula">
       <calculatedColumnFormula>D2-B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Data final" dataDxfId="14" totalsRowDxfId="13" dataCellStyle="Vírgula"/>
-    <tableColumn id="8" name="Descrição" dataDxfId="0" totalsRowDxfId="1" dataCellStyle="Vírgula"/>
-    <tableColumn id="5" name="DiaI" dataDxfId="12" totalsRowDxfId="11">
+    <tableColumn id="4" name="Data final" dataDxfId="15" totalsRowDxfId="14" dataCellStyle="Vírgula"/>
+    <tableColumn id="8" name="Descrição" dataDxfId="13" totalsRowDxfId="12" dataCellStyle="Vírgula"/>
+    <tableColumn id="5" name="DiaI" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>DAY(Tabela1[[#This Row],[Data inicial]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="MêsI" dataDxfId="10" totalsRowDxfId="9">
+    <tableColumn id="6" name="MêsI" dataDxfId="9" totalsRowDxfId="8">
       <calculatedColumnFormula>MONTH(Tabela1[[#This Row],[Data inicial]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="AnoI" dataDxfId="8" totalsRowDxfId="7">
+    <tableColumn id="7" name="AnoI" dataDxfId="7" totalsRowDxfId="6">
       <calculatedColumnFormula>YEAR(Tabela1[[#This Row],[Data inicial]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2583,18 +2695,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="I1:K20" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="I1:K20"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="DiaF" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="I1:L20" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="I1:L20"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="DiaF" dataDxfId="3">
       <calculatedColumnFormula>DAY(Tabela1[[#This Row],[Data final]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="MêsF" dataDxfId="3">
+    <tableColumn id="2" name="MêsF" dataDxfId="2">
       <calculatedColumnFormula>MONTH(Tabela1[[#This Row],[Data final]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="AnoF" dataDxfId="2">
+    <tableColumn id="3" name="AnoF" dataDxfId="1">
       <calculatedColumnFormula>YEAR(Tabela1[[#This Row],[Data final]])</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="4" name="Color" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2866,10 +2979,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2882,10 +2995,11 @@
     <col min="6" max="6" width="17.140625" style="1" customWidth="1"/>
     <col min="7" max="8" width="9.140625" style="1"/>
     <col min="9" max="11" width="10.28515625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="12" width="21.5703125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -2919,12 +3033,15 @@
       <c r="K1" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="L1" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="17">
         <v>41845</v>
       </c>
       <c r="C2" s="5">
@@ -2951,7 +3068,7 @@
       </c>
       <c r="I2" s="12">
         <f>I14</f>
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="J2" s="12">
         <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
@@ -2961,20 +3078,23 @@
         <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
         <v>2017</v>
       </c>
+      <c r="L2" s="20" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="17">
         <v>41845</v>
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:C12" si="0">D3-B3</f>
-        <v>1175</v>
+        <v>810</v>
       </c>
       <c r="D3" s="4">
-        <v>43020</v>
+        <v>42655</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="11">
@@ -2999,22 +3119,25 @@
       </c>
       <c r="K3" s="12">
         <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
-        <v>2017</v>
+        <v>2016</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="17">
         <v>42248</v>
       </c>
       <c r="C4" s="5">
         <f t="shared" si="0"/>
-        <v>791</v>
+        <v>121</v>
       </c>
       <c r="D4" s="4">
-        <v>43039</v>
+        <v>42369</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="11">
@@ -3035,18 +3158,21 @@
       </c>
       <c r="J4" s="12">
         <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K4" s="12">
         <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
-        <v>2017</v>
+        <v>2015</v>
+      </c>
+      <c r="L4" s="21" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="17">
         <v>42371</v>
       </c>
       <c r="C5" s="5">
@@ -3081,20 +3207,23 @@
         <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
         <v>2017</v>
       </c>
+      <c r="L5" s="21" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="17">
         <v>41845</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" si="0"/>
-        <v>1194</v>
+        <v>69</v>
       </c>
       <c r="D6" s="4">
-        <v>43039</v>
+        <v>41914</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="11">
@@ -3111,7 +3240,7 @@
       </c>
       <c r="I6" s="12">
         <f>DAY(Tabela1[[#This Row],[Data final]])</f>
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="J6" s="12">
         <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
@@ -3119,22 +3248,25 @@
       </c>
       <c r="K6" s="12">
         <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
-        <v>2017</v>
+        <v>2014</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="17">
         <v>41883</v>
       </c>
       <c r="C7" s="5">
         <f t="shared" si="0"/>
-        <v>1156</v>
+        <v>121</v>
       </c>
       <c r="D7" s="4">
-        <v>43039</v>
+        <v>42004</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="11">
@@ -3155,26 +3287,29 @@
       </c>
       <c r="J7" s="12">
         <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K7" s="12">
         <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
-        <v>2017</v>
+        <v>2014</v>
+      </c>
+      <c r="L7" s="21" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="17">
         <v>41640</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" si="0"/>
-        <v>1399</v>
+        <v>607</v>
       </c>
       <c r="D8" s="4">
-        <v>43039</v>
+        <v>42247</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="11">
@@ -3195,26 +3330,29 @@
       </c>
       <c r="J8" s="12">
         <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K8" s="12">
         <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
-        <v>2017</v>
+        <v>2015</v>
+      </c>
+      <c r="L8" s="21" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="17">
         <v>41845</v>
       </c>
       <c r="C9" s="5">
         <f t="shared" si="0"/>
-        <v>1194</v>
+        <v>98</v>
       </c>
       <c r="D9" s="4">
-        <v>43039</v>
+        <v>41943</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="11">
@@ -3239,22 +3377,25 @@
       </c>
       <c r="K9" s="12">
         <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
-        <v>2017</v>
+        <v>2014</v>
+      </c>
+      <c r="L9" s="21" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="17">
         <v>41845</v>
       </c>
       <c r="C10" s="5">
         <f t="shared" si="0"/>
-        <v>1194</v>
+        <v>921</v>
       </c>
       <c r="D10" s="4">
-        <v>43039</v>
+        <v>42766</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="11">
@@ -3275,26 +3416,29 @@
       </c>
       <c r="J10" s="12">
         <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K10" s="12">
         <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
         <v>2017</v>
       </c>
+      <c r="L10" s="21" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="17">
         <v>42309</v>
       </c>
       <c r="C11" s="5">
         <f t="shared" si="0"/>
-        <v>730</v>
+        <v>373</v>
       </c>
       <c r="D11" s="4">
-        <v>43039</v>
+        <v>42682</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>24</v>
@@ -3313,30 +3457,33 @@
       </c>
       <c r="I11" s="12">
         <f>DAY(Tabela1[[#This Row],[Data final]])</f>
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="J11" s="12">
         <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K11" s="12">
         <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
-        <v>2017</v>
+        <v>2016</v>
+      </c>
+      <c r="L11" s="19" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="17">
         <v>41276</v>
       </c>
       <c r="C12" s="5">
         <f t="shared" si="0"/>
-        <v>1763</v>
+        <v>1610</v>
       </c>
       <c r="D12" s="4">
-        <v>43039</v>
+        <v>42886</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>25</v>
@@ -3359,26 +3506,29 @@
       </c>
       <c r="J12" s="12">
         <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K12" s="12">
         <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
         <v>2017</v>
       </c>
+      <c r="L12" s="23" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="17">
         <v>41845</v>
       </c>
       <c r="C13" s="5">
         <f t="shared" ref="C13" si="1">D13-B13</f>
-        <v>1194</v>
+        <v>829</v>
       </c>
       <c r="D13" s="4">
-        <v>43039</v>
+        <v>42674</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="11">
@@ -3403,22 +3553,25 @@
       </c>
       <c r="K13" s="12">
         <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
-        <v>2017</v>
+        <v>2016</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="17">
         <v>41845</v>
       </c>
       <c r="C14" s="5">
         <f t="shared" ref="C14" si="2">D14-B14</f>
-        <v>1194</v>
+        <v>1477</v>
       </c>
       <c r="D14" s="4">
-        <v>43039</v>
+        <v>43322</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>26</v>
@@ -3437,18 +3590,21 @@
       </c>
       <c r="I14" s="12">
         <f>DAY(Tabela1[[#This Row],[Data final]])</f>
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="J14" s="12">
         <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K14" s="12">
         <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
-        <v>2017</v>
+        <v>2018</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="12" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" s="12" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -3456,8 +3612,9 @@
       <c r="E15" s="15"/>
       <c r="F15" s="11"/>
       <c r="H15" s="13"/>
+      <c r="L15" s="16"/>
     </row>
-    <row r="16" spans="1:11" s="12" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" s="12" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
@@ -3465,8 +3622,9 @@
       <c r="E16" s="15"/>
       <c r="F16" s="11"/>
       <c r="H16" s="13"/>
+      <c r="L16" s="16"/>
     </row>
-    <row r="17" spans="1:11" s="12" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" s="12" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="3"/>
       <c r="C17" s="5"/>
@@ -3474,8 +3632,9 @@
       <c r="E17" s="15"/>
       <c r="F17" s="11"/>
       <c r="H17" s="13"/>
+      <c r="L17" s="16"/>
     </row>
-    <row r="18" spans="1:11" s="12" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" s="12" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="3"/>
       <c r="C18" s="5"/>
@@ -3483,8 +3642,9 @@
       <c r="E18" s="15"/>
       <c r="F18" s="11"/>
       <c r="H18" s="13"/>
+      <c r="L18" s="16"/>
     </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" s="12" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
@@ -3492,8 +3652,9 @@
       <c r="E19" s="15"/>
       <c r="F19" s="11"/>
       <c r="H19" s="13"/>
+      <c r="L19" s="16"/>
     </row>
-    <row r="20" spans="1:11" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
@@ -3501,8 +3662,9 @@
       <c r="E20" s="15"/>
       <c r="F20" s="11"/>
       <c r="H20" s="13"/>
+      <c r="L20" s="16"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -3515,7 +3677,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -3528,7 +3690,7 @@
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>

</xml_diff>

<commit_message>
change for red lines
</commit_message>
<xml_diff>
--- a/excel/modelo_linha_do_tempo.xlsx
+++ b/excel/modelo_linha_do_tempo.xlsx
@@ -2463,11 +2463,11 @@
         </c:dLbls>
         <c:gapWidth val="10"/>
         <c:overlap val="100"/>
-        <c:axId val="121040080"/>
-        <c:axId val="351978816"/>
+        <c:axId val="384003544"/>
+        <c:axId val="384003928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="121040080"/>
+        <c:axId val="384003544"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2521,7 +2521,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351978816"/>
+        <c:crossAx val="384003928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2529,7 +2529,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="351978816"/>
+        <c:axId val="384003928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43466"/>
@@ -2579,7 +2579,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121040080"/>
+        <c:crossAx val="384003544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="366"/>
@@ -2646,7 +2646,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{52BF227D-3AC3-4B5A-88A9-8F410E929E4B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52BF227D-3AC3-4B5A-88A9-8F410E929E4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2982,7 +2982,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="A3" sqref="A3:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Stripes | Is Board Some Name inputed
</commit_message>
<xml_diff>
--- a/excel/modelo_linha_do_tempo.xlsx
+++ b/excel/modelo_linha_do_tempo.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>E</t>
   </si>
@@ -49,9 +49,6 @@
     <t>H</t>
   </si>
   <si>
-    <t>I</t>
-  </si>
-  <si>
     <t>J</t>
   </si>
   <si>
@@ -115,9 +112,6 @@
     <t>Programar</t>
   </si>
   <si>
-    <t>Robando e Mentindo</t>
-  </si>
-  <si>
     <t>Color</t>
   </si>
   <si>
@@ -137,6 +131,27 @@
   </si>
   <si>
     <t>255,0,0</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>Desenhar</t>
+  </si>
+  <si>
+    <t>155,194,230</t>
+  </si>
+  <si>
+    <t>Robando e Mentir</t>
+  </si>
+  <si>
+    <t>Ze Ninguem</t>
+  </si>
+  <si>
+    <t>Stripes</t>
+  </si>
+  <si>
+    <t>Enable</t>
   </si>
 </sst>
 </file>
@@ -210,7 +225,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +271,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -312,7 +339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -379,12 +406,43 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1087,7 +1145,7 @@
             <c:strRef>
               <c:f>'Linhas do tempo'!$A$2:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Danilaw</c:v>
                 </c:pt>
@@ -1104,7 +1162,7 @@
                   <c:v>H</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>I</c:v>
+                  <c:v>Ivan</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>J</c:v>
@@ -1113,7 +1171,7 @@
                   <c:v>K</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>L</c:v>
+                  <c:v>Ze Ninguem</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Marina</c:v>
@@ -1126,6 +1184,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Leonardo Rouba Dinheiro</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Ze Ninguem</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1158,9 +1219,6 @@
                   <c:v>41640</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41845</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>41845</c:v>
                 </c:pt>
                 <c:pt idx="9">
@@ -1245,7 +1303,7 @@
             <c:strRef>
               <c:f>'Linhas do tempo'!$A$2:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Danilaw</c:v>
                 </c:pt>
@@ -1262,7 +1320,7 @@
                   <c:v>H</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>I</c:v>
+                  <c:v>Ivan</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>J</c:v>
@@ -1271,7 +1329,7 @@
                   <c:v>K</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>L</c:v>
+                  <c:v>Ze Ninguem</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Marina</c:v>
@@ -1284,6 +1342,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Leonardo Rouba Dinheiro</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Ze Ninguem</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1310,16 +1371,13 @@
                   <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>121</c:v>
+                  <c:v>852</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>607</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>921</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>373</c:v>
@@ -1361,7 +1419,7 @@
             <c:strRef>
               <c:f>'Linhas do tempo'!$A$2:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Danilaw</c:v>
                 </c:pt>
@@ -1378,7 +1436,7 @@
                   <c:v>H</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>I</c:v>
+                  <c:v>Ivan</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>J</c:v>
@@ -1387,7 +1445,7 @@
                   <c:v>K</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>L</c:v>
+                  <c:v>Ze Ninguem</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Marina</c:v>
@@ -1400,6 +1458,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Leonardo Rouba Dinheiro</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Ze Ninguem</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1432,9 +1493,6 @@
                   <c:v>41640</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41845</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>41845</c:v>
                 </c:pt>
                 <c:pt idx="9">
@@ -1519,7 +1577,7 @@
             <c:strRef>
               <c:f>'Linhas do tempo'!$A$2:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Danilaw</c:v>
                 </c:pt>
@@ -1536,7 +1594,7 @@
                   <c:v>H</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>I</c:v>
+                  <c:v>Ivan</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>J</c:v>
@@ -1545,7 +1603,7 @@
                   <c:v>K</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>L</c:v>
+                  <c:v>Ze Ninguem</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Marina</c:v>
@@ -1558,6 +1616,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Leonardo Rouba Dinheiro</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Ze Ninguem</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1584,16 +1645,13 @@
                   <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>121</c:v>
+                  <c:v>852</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>607</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>921</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>373</c:v>
@@ -1635,7 +1693,7 @@
             <c:strRef>
               <c:f>'Linhas do tempo'!$A$2:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Danilaw</c:v>
                 </c:pt>
@@ -1652,7 +1710,7 @@
                   <c:v>H</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>I</c:v>
+                  <c:v>Ivan</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>J</c:v>
@@ -1661,7 +1719,7 @@
                   <c:v>K</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>L</c:v>
+                  <c:v>Ze Ninguem</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Marina</c:v>
@@ -1674,6 +1732,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Leonardo Rouba Dinheiro</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Ze Ninguem</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1706,9 +1767,6 @@
                   <c:v>41640</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41845</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>41845</c:v>
                 </c:pt>
                 <c:pt idx="9">
@@ -1793,7 +1851,7 @@
             <c:strRef>
               <c:f>'Linhas do tempo'!$A$2:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Danilaw</c:v>
                 </c:pt>
@@ -1810,7 +1868,7 @@
                   <c:v>H</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>I</c:v>
+                  <c:v>Ivan</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>J</c:v>
@@ -1819,7 +1877,7 @@
                   <c:v>K</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>L</c:v>
+                  <c:v>Ze Ninguem</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Marina</c:v>
@@ -1832,6 +1890,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Leonardo Rouba Dinheiro</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Ze Ninguem</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1858,16 +1919,13 @@
                   <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>121</c:v>
+                  <c:v>852</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>607</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>921</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>373</c:v>
@@ -1916,7 +1974,7 @@
             <c:strRef>
               <c:f>'Linhas do tempo'!$A$2:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Danilaw</c:v>
                 </c:pt>
@@ -1933,7 +1991,7 @@
                   <c:v>H</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>I</c:v>
+                  <c:v>Ivan</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>J</c:v>
@@ -1942,7 +2000,7 @@
                   <c:v>K</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>L</c:v>
+                  <c:v>Ze Ninguem</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Marina</c:v>
@@ -1955,6 +2013,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Leonardo Rouba Dinheiro</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Ze Ninguem</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1987,9 +2048,6 @@
                   <c:v>41640</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41845</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>41845</c:v>
                 </c:pt>
                 <c:pt idx="9">
@@ -2356,7 +2414,7 @@
             <c:strRef>
               <c:f>'Linhas do tempo'!$A$2:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Danilaw</c:v>
                 </c:pt>
@@ -2373,7 +2431,7 @@
                   <c:v>H</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>I</c:v>
+                  <c:v>Ivan</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>J</c:v>
@@ -2382,7 +2440,7 @@
                   <c:v>K</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>L</c:v>
+                  <c:v>Ze Ninguem</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Marina</c:v>
@@ -2395,6 +2453,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Leonardo Rouba Dinheiro</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Ze Ninguem</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2421,16 +2482,13 @@
                   <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>121</c:v>
+                  <c:v>852</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>607</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>921</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>373</c:v>
@@ -2463,11 +2521,11 @@
         </c:dLbls>
         <c:gapWidth val="10"/>
         <c:overlap val="100"/>
-        <c:axId val="384003544"/>
-        <c:axId val="384003928"/>
+        <c:axId val="400191288"/>
+        <c:axId val="350617680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="384003544"/>
+        <c:axId val="400191288"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2521,7 +2579,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384003928"/>
+        <c:crossAx val="350617680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2529,7 +2587,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="384003928"/>
+        <c:axId val="350617680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43466"/>
@@ -2579,7 +2637,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384003544"/>
+        <c:crossAx val="400191288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="366"/>
@@ -2630,16 +2688,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>257175</xdr:rowOff>
+      <xdr:rowOff>323850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2670,23 +2728,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:H20" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:H20" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" tableBorderDxfId="23">
   <autoFilter ref="A1:H20"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Evento" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="2" name="Data inicial" dataDxfId="19" totalsRowDxfId="18" dataCellStyle="Vírgula"/>
-    <tableColumn id="3" name="Duração em dias" dataDxfId="17" totalsRowDxfId="16" dataCellStyle="Vírgula">
+    <tableColumn id="1" name="Evento" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="2" name="Data inicial" dataDxfId="20" totalsRowDxfId="19" dataCellStyle="Vírgula"/>
+    <tableColumn id="3" name="Duração em dias" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Vírgula">
       <calculatedColumnFormula>D2-B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Data final" dataDxfId="15" totalsRowDxfId="14" dataCellStyle="Vírgula"/>
-    <tableColumn id="8" name="Descrição" dataDxfId="13" totalsRowDxfId="12" dataCellStyle="Vírgula"/>
-    <tableColumn id="5" name="DiaI" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="4" name="Data final" dataDxfId="16" totalsRowDxfId="15" dataCellStyle="Vírgula"/>
+    <tableColumn id="8" name="Descrição" dataDxfId="14" totalsRowDxfId="13" dataCellStyle="Vírgula"/>
+    <tableColumn id="5" name="DiaI" dataDxfId="12" totalsRowDxfId="11">
       <calculatedColumnFormula>DAY(Tabela1[[#This Row],[Data inicial]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="MêsI" dataDxfId="9" totalsRowDxfId="8">
+    <tableColumn id="6" name="MêsI" dataDxfId="10" totalsRowDxfId="9">
       <calculatedColumnFormula>MONTH(Tabela1[[#This Row],[Data inicial]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="AnoI" dataDxfId="7" totalsRowDxfId="6">
+    <tableColumn id="7" name="AnoI" dataDxfId="8" totalsRowDxfId="7">
       <calculatedColumnFormula>YEAR(Tabela1[[#This Row],[Data inicial]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2695,19 +2753,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="I1:L20" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="I1:L20"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="DiaF" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="I1:M20" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="I1:M20"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="DiaF" dataDxfId="4">
       <calculatedColumnFormula>DAY(Tabela1[[#This Row],[Data final]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="MêsF" dataDxfId="2">
+    <tableColumn id="2" name="MêsF" dataDxfId="3">
       <calculatedColumnFormula>MONTH(Tabela1[[#This Row],[Data final]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="AnoF" dataDxfId="1">
+    <tableColumn id="3" name="AnoF" dataDxfId="2">
       <calculatedColumnFormula>YEAR(Tabela1[[#This Row],[Data final]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Color" dataDxfId="0"/>
+    <tableColumn id="4" name="Color" dataDxfId="1"/>
+    <tableColumn id="5" name="Stripes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2979,10 +3038,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2999,47 +3058,50 @@
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>12</v>
       </c>
       <c r="B2" s="17">
         <v>41845</v>
@@ -3052,7 +3114,7 @@
         <v>43039</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="11">
         <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
@@ -3079,10 +3141,13 @@
         <v>2017</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -3122,10 +3187,11 @@
         <v>2016</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>29</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="M3" s="25"/>
     </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
@@ -3165,10 +3231,11 @@
         <v>2015</v>
       </c>
       <c r="L4" s="21" t="s">
-        <v>29</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="M4" s="25"/>
     </row>
-    <row r="5" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
@@ -3208,10 +3275,11 @@
         <v>2017</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>29</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="M5" s="25"/>
     </row>
-    <row r="6" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
@@ -3251,24 +3319,27 @@
         <v>2014</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>29</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="M6" s="25"/>
     </row>
-    <row r="7" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B7" s="17">
         <v>41883</v>
       </c>
       <c r="C7" s="5">
         <f t="shared" si="0"/>
-        <v>121</v>
+        <v>852</v>
       </c>
       <c r="D7" s="4">
-        <v>42004</v>
-      </c>
-      <c r="E7" s="15"/>
+        <v>42735</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="F7" s="11">
         <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
         <v>1</v>
@@ -3291,15 +3362,18 @@
       </c>
       <c r="K7" s="12">
         <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
-        <v>2014</v>
-      </c>
-      <c r="L7" s="21" t="s">
-        <v>29</v>
+        <v>2016</v>
+      </c>
+      <c r="L7" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="17">
         <v>41640</v>
@@ -3337,12 +3411,13 @@
         <v>2015</v>
       </c>
       <c r="L8" s="21" t="s">
-        <v>29</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="M8" s="25"/>
     </row>
-    <row r="9" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="17">
         <v>41845</v>
@@ -3380,55 +3455,30 @@
         <v>2014</v>
       </c>
       <c r="L9" s="21" t="s">
-        <v>29</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="M9" s="25"/>
     </row>
-    <row r="10" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="17">
-        <v>41845</v>
-      </c>
-      <c r="C10" s="5">
-        <f t="shared" si="0"/>
-        <v>921</v>
-      </c>
-      <c r="D10" s="4">
-        <v>42766</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="4"/>
       <c r="E10" s="15"/>
-      <c r="F10" s="11">
-        <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
-        <v>25</v>
-      </c>
-      <c r="G10" s="12">
-        <f>MONTH(Tabela1[[#This Row],[Data inicial]])</f>
-        <v>7</v>
-      </c>
-      <c r="H10" s="13">
-        <f>YEAR(Tabela1[[#This Row],[Data inicial]])</f>
-        <v>2014</v>
-      </c>
-      <c r="I10" s="12">
-        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
-        <v>31</v>
-      </c>
-      <c r="J10" s="12">
-        <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
-        <v>1</v>
-      </c>
-      <c r="K10" s="12">
-        <f>YEAR(Tabela1[[#This Row],[Data final]])</f>
-        <v>2017</v>
-      </c>
-      <c r="L10" s="21" t="s">
-        <v>29</v>
-      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="25"/>
     </row>
-    <row r="11" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="17">
         <v>42309</v>
@@ -3441,7 +3491,7 @@
         <v>42682</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="11">
         <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
@@ -3468,12 +3518,13 @@
         <v>2016</v>
       </c>
       <c r="L11" s="19" t="s">
-        <v>30</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="M11" s="25"/>
     </row>
-    <row r="12" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="17">
         <v>41276</v>
@@ -3486,7 +3537,7 @@
         <v>42886</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="11">
         <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
@@ -3513,12 +3564,13 @@
         <v>2017</v>
       </c>
       <c r="L12" s="23" t="s">
-        <v>31</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="M12" s="25"/>
     </row>
-    <row r="13" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="17">
         <v>41845</v>
@@ -3556,12 +3608,13 @@
         <v>2016</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>32</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="M13" s="25"/>
     </row>
-    <row r="14" spans="1:12" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="17">
         <v>41845</v>
@@ -3574,7 +3627,7 @@
         <v>43322</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F14" s="11">
         <f>DAY(Tabela1[[#This Row],[Data inicial]])</f>
@@ -3601,30 +3654,43 @@
         <v>2018</v>
       </c>
       <c r="L14" s="18" t="s">
-        <v>33</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="M14" s="25"/>
     </row>
-    <row r="15" spans="1:12" s="12" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="4"/>
+    <row r="15" spans="1:13" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="17"/>
       <c r="C15" s="5"/>
       <c r="D15" s="4"/>
       <c r="E15" s="15"/>
       <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
       <c r="H15" s="13"/>
-      <c r="L15" s="16"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="25"/>
     </row>
-    <row r="16" spans="1:12" s="12" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
-      <c r="B16" s="4"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="5"/>
       <c r="D16" s="4"/>
       <c r="E16" s="15"/>
       <c r="F16" s="11"/>
+      <c r="G16" s="12"/>
       <c r="H16" s="13"/>
-      <c r="L16" s="16"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="25"/>
     </row>
-    <row r="17" spans="1:12" s="12" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" s="12" customFormat="1" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="3"/>
       <c r="C17" s="5"/>
@@ -3632,19 +3698,25 @@
       <c r="E17" s="15"/>
       <c r="F17" s="11"/>
       <c r="H17" s="13"/>
-      <c r="L17" s="16"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="25"/>
     </row>
-    <row r="18" spans="1:12" s="12" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
-      <c r="B18" s="3"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="5"/>
       <c r="D18" s="4"/>
       <c r="E18" s="15"/>
       <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
       <c r="H18" s="13"/>
-      <c r="L18" s="16"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="25"/>
     </row>
-    <row r="19" spans="1:12" s="12" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" s="12" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
@@ -3653,8 +3725,9 @@
       <c r="F19" s="11"/>
       <c r="H19" s="13"/>
       <c r="L19" s="16"/>
+      <c r="M19" s="25"/>
     </row>
-    <row r="20" spans="1:12" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" s="12" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
@@ -3663,8 +3736,9 @@
       <c r="F20" s="11"/>
       <c r="H20" s="13"/>
       <c r="L20" s="16"/>
+      <c r="M20" s="25"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -3677,7 +3751,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -3690,7 +3764,7 @@
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>

</xml_diff>

<commit_message>
Initial Data - Final Data
</commit_message>
<xml_diff>
--- a/excel/modelo_linha_do_tempo.xlsx
+++ b/excel/modelo_linha_do_tempo.xlsx
@@ -457,7 +457,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -475,26 +475,6 @@
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -531,7 +511,27 @@
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2736,11 +2736,11 @@
         </c:dLbls>
         <c:gapWidth val="10"/>
         <c:overlap val="100"/>
-        <c:axId val="354548904"/>
-        <c:axId val="354546552"/>
+        <c:axId val="353996320"/>
+        <c:axId val="401287592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="354548904"/>
+        <c:axId val="353996320"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2794,7 +2794,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354546552"/>
+        <c:crossAx val="401287592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2802,7 +2802,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="354546552"/>
+        <c:axId val="401287592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43466"/>
@@ -2852,7 +2852,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354548904"/>
+        <c:crossAx val="353996320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="366"/>
@@ -2919,7 +2919,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{52BF227D-3AC3-4B5A-88A9-8F410E929E4B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52BF227D-3AC3-4B5A-88A9-8F410E929E4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2980,18 +2980,18 @@
     <tableColumn id="3" name="AnoF" dataDxfId="5">
       <calculatedColumnFormula>YEAR(Tabela1[[#This Row],[Data final]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Color" dataDxfId="1"/>
-    <tableColumn id="5" name="Stripes" dataDxfId="0"/>
+    <tableColumn id="4" name="Color" dataDxfId="4"/>
+    <tableColumn id="5" name="Stripes" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:A19" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:A19" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="A1:A19"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="ID" dataDxfId="2">
+    <tableColumn id="1" name="ID" dataDxfId="0">
       <calculatedColumnFormula>ROW()</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3268,7 +3268,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3999,8 +3999,8 @@
         <v>2015</v>
       </c>
       <c r="J16" s="11">
-        <f>J28</f>
-        <v>0</v>
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>31</v>
       </c>
       <c r="K16" s="11">
         <f>MONTH(Tabela1[[#This Row],[Data final]])</f>
@@ -4050,8 +4050,8 @@
         <v>2016</v>
       </c>
       <c r="J17" s="11">
-        <f>J29</f>
-        <v>0</v>
+        <f>DAY(Tabela1[[#This Row],[Data final]])</f>
+        <v>31</v>
       </c>
       <c r="K17" s="11">
         <f>MONTH(Tabela1[[#This Row],[Data final]])</f>

</xml_diff>